<commit_message>
Zostal wstep, zakonczenie i formatowanie
</commit_message>
<xml_diff>
--- a/Notatka/Tab/podprobkowanie.xlsx
+++ b/Notatka/Tab/podprobkowanie.xlsx
@@ -29,6 +29,113 @@
     <t>m</t>
   </si>
   <si>
+    <t>L.p.</t>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [kHz]</t>
+    </r>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <r>
+      <t>Δf</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [Hz]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s_min</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(m) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[kHz]</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>f</t>
     </r>
@@ -66,114 +173,7 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>[Hz]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s_min</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(m) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Hz]</t>
-    </r>
-  </si>
-  <si>
-    <t>L.p.</t>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [kHz]</t>
-    </r>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <r>
-      <t>Δf</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> [Hz]</t>
+      <t>[kHz]</t>
     </r>
   </si>
 </sst>
@@ -181,11 +181,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000000"/>
-    <numFmt numFmtId="167" formatCode="0.000000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000000"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -269,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -283,16 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,7 +571,7 @@
   <dimension ref="A5:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="A50" sqref="A50:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,10 +585,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -608,12 +596,12 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B27" si="0">G6/(A6 + 1)</f>
-        <v>3185000</v>
+        <f>(G6/(A6 + 1))/1000</f>
+        <v>3185</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C27" si="1">F6/A6</f>
-        <v>6070000</v>
+        <f>(F6/A6)/1000</f>
+        <v>6070</v>
       </c>
       <c r="F6">
         <v>6070000</v>
@@ -627,12 +615,12 @@
         <v>2</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>2123333.3333333335</v>
+        <f t="shared" ref="B7:B27" si="0">(G7/(A7 + 1))/1000</f>
+        <v>2123.3333333333335</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
-        <v>3035000</v>
+        <f t="shared" ref="C7:C27" si="1">(F7/A7)/1000</f>
+        <v>3035</v>
       </c>
       <c r="F7">
         <v>6070000</v>
@@ -647,11 +635,11 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>1592500</v>
+        <v>1592.5</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>2023333.3333333333</v>
+        <v>2023.3333333333333</v>
       </c>
       <c r="F8">
         <v>6070000</v>
@@ -666,11 +654,11 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>1274000</v>
+        <v>1274</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>1517500</v>
+        <v>1517.5</v>
       </c>
       <c r="F9">
         <v>6070000</v>
@@ -685,11 +673,11 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>1061666.6666666667</v>
+        <v>1061.6666666666667</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>1214000</v>
+        <v>1214</v>
       </c>
       <c r="F10">
         <v>6070000</v>
@@ -704,11 +692,11 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>910000</v>
+        <v>910</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>1011666.6666666666</v>
+        <v>1011.6666666666666</v>
       </c>
       <c r="F11">
         <v>6070000</v>
@@ -723,11 +711,11 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>796250</v>
+        <v>796.25</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>867142.85714285716</v>
+        <v>867.14285714285711</v>
       </c>
       <c r="F12">
         <v>6070000</v>
@@ -742,11 +730,11 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>707777.77777777775</v>
+        <v>707.77777777777771</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>758750</v>
+        <v>758.75</v>
       </c>
       <c r="F13">
         <v>6070000</v>
@@ -761,11 +749,11 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>637000</v>
+        <v>637</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>674444.4444444445</v>
+        <v>674.44444444444446</v>
       </c>
       <c r="F14">
         <v>6070000</v>
@@ -780,11 +768,11 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>579090.90909090906</v>
+        <v>579.09090909090901</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>607000</v>
+        <v>607</v>
       </c>
       <c r="F15">
         <v>6070000</v>
@@ -799,11 +787,11 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>530833.33333333337</v>
+        <v>530.83333333333337</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>551818.18181818177</v>
+        <v>551.81818181818176</v>
       </c>
       <c r="F16">
         <v>6070000</v>
@@ -818,11 +806,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>490000</v>
+        <v>490</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>505833.33333333331</v>
+        <v>505.83333333333331</v>
       </c>
       <c r="F17">
         <v>6070000</v>
@@ -837,11 +825,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>455000</v>
+        <v>455</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>466923.07692307694</v>
+        <v>466.92307692307696</v>
       </c>
       <c r="F18">
         <v>6070000</v>
@@ -856,11 +844,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>424666.66666666669</v>
+        <v>424.66666666666669</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>433571.42857142858</v>
+        <v>433.57142857142856</v>
       </c>
       <c r="F19">
         <v>6070000</v>
@@ -875,11 +863,11 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>398125</v>
+        <v>398.125</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="1"/>
-        <v>404666.66666666669</v>
+        <v>404.66666666666669</v>
       </c>
       <c r="F20">
         <v>6070000</v>
@@ -894,11 +882,11 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>374705.8823529412</v>
+        <v>374.70588235294122</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="1"/>
-        <v>379375</v>
+        <v>379.375</v>
       </c>
       <c r="F21">
         <v>6070000</v>
@@ -913,11 +901,11 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>353888.88888888888</v>
+        <v>353.88888888888886</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="1"/>
-        <v>357058.82352941175</v>
+        <v>357.05882352941177</v>
       </c>
       <c r="F22">
         <v>6070000</v>
@@ -932,11 +920,11 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>335263.15789473685</v>
+        <v>335.26315789473688</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="1"/>
-        <v>337222.22222222225</v>
+        <v>337.22222222222223</v>
       </c>
       <c r="F23">
         <v>6070000</v>
@@ -951,11 +939,11 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>318500</v>
+        <v>318.5</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="1"/>
-        <v>319473.68421052629</v>
+        <v>319.4736842105263</v>
       </c>
       <c r="F24">
         <v>6070000</v>
@@ -970,11 +958,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>303333.33333333331</v>
+        <v>303.33333333333331</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="1"/>
-        <v>303500</v>
+        <v>303.5</v>
       </c>
       <c r="F25">
         <v>6070000</v>
@@ -988,12 +976,12 @@
         <v>21</v>
       </c>
       <c r="B26" s="4">
-        <f t="shared" si="0"/>
-        <v>289545.45454545453</v>
+        <f>(G26/(A26 + 1))/1000</f>
+        <v>289.5454545454545</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>289047.61904761905</v>
+        <v>289.04761904761904</v>
       </c>
       <c r="F26">
         <v>6070000</v>
@@ -1008,11 +996,11 @@
       </c>
       <c r="B27" s="4">
         <f t="shared" si="0"/>
-        <v>276956.52173913043</v>
+        <v>276.95652173913044</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>275909.09090909088</v>
+        <v>275.90909090909088</v>
       </c>
       <c r="F27">
         <v>6070000</v>
@@ -1023,10 +1011,10 @@
     </row>
     <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1143,10 +1131,10 @@
     </row>
     <row r="50" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1154,35 +1142,35 @@
         <v>1024</v>
       </c>
       <c r="B51" s="5">
-        <f>319000/A51</f>
-        <v>311.5234375</v>
+        <f>400000/A51</f>
+        <v>390.625</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>2048</v>
       </c>
-      <c r="B52" s="6">
-        <f t="shared" ref="B52:B54" si="2">319000/A52</f>
-        <v>155.76171875</v>
+      <c r="B52" s="5">
+        <f t="shared" ref="B52:B54" si="2">400000/A52</f>
+        <v>195.3125</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>4096</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="5">
         <f t="shared" si="2"/>
-        <v>77.880859375</v>
+        <v>97.65625</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>8192</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="5">
         <f t="shared" si="2"/>
-        <v>38.9404296875</v>
+        <v>48.828125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>